<commit_message>
Updated test case list with additional importBallotsHeader test cases
</commit_message>
<xml_diff>
--- a/Project2/testing/Test Case List.xlsx
+++ b/Project2/testing/Test Case List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nik312123/git/repo-Team19/Project1/testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nik312123/git/repo-Team19/Project2/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{929E1083-B28B-2F44-855F-ED4428D68377}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED2A0EA1-CA78-9F49-91D7-CF9E69C9DF6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="474">
   <si>
     <t>Class Name</t>
   </si>
@@ -1409,37 +1409,40 @@
     <t>testOplTime1</t>
   </si>
   <si>
+    <t>testOplTime4</t>
+  </si>
+  <si>
+    <t>testOplTime16</t>
+  </si>
+  <si>
+    <t>testOplTime64</t>
+  </si>
+  <si>
+    <t>testOplTime256</t>
+  </si>
+  <si>
+    <t>testOplTime1024</t>
+  </si>
+  <si>
+    <t>testOplTime4096</t>
+  </si>
+  <si>
+    <t>testOplTime16384</t>
+  </si>
+  <si>
+    <t>testOplTime65536</t>
+  </si>
+  <si>
+    <t>testOplTime262144</t>
+  </si>
+  <si>
+    <t>testRunElectionTwoCandidateMajority</t>
+  </si>
+  <si>
     <t>testRunElectionTieBreaksOutput</t>
   </si>
   <si>
-    <t>testOplTime4</t>
-  </si>
-  <si>
-    <t>testOplTime16</t>
-  </si>
-  <si>
-    <t>testOplTime64</t>
-  </si>
-  <si>
-    <t>testOplTime256</t>
-  </si>
-  <si>
-    <t>testOplTime1024</t>
-  </si>
-  <si>
-    <t>testOplTime4096</t>
-  </si>
-  <si>
-    <t>testOplTime16384</t>
-  </si>
-  <si>
-    <t>testOplTime65536</t>
-  </si>
-  <si>
-    <t>testOplTime262144</t>
-  </si>
-  <si>
-    <t>testRunElectionTwoCandidateMajority</t>
+    <t>testMultipleImports</t>
   </si>
   <si>
     <t>Test Case #</t>
@@ -1925,22 +1928,22 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z449"/>
+  <dimension ref="A1:Z451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A395" workbookViewId="0">
-      <selection activeCell="I416" sqref="I416"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="39.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="57.5" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
     <col min="10" max="10" width="39" customWidth="1"/>
     <col min="11" max="11" width="19.83203125" customWidth="1"/>
@@ -2293,7 +2296,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>12</v>
@@ -21431,7 +21434,7 @@
         <v>9</v>
       </c>
       <c r="G438" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H438" s="11" t="s">
         <v>20</v>
@@ -21476,7 +21479,7 @@
         <v>10</v>
       </c>
       <c r="G439" s="14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H439" s="14" t="s">
         <v>20</v>
@@ -21521,7 +21524,7 @@
         <v>11</v>
       </c>
       <c r="G440" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H440" s="11" t="s">
         <v>20</v>
@@ -21566,7 +21569,7 @@
         <v>12</v>
       </c>
       <c r="G441" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H441" s="14" t="s">
         <v>20</v>
@@ -21611,7 +21614,7 @@
         <v>13</v>
       </c>
       <c r="G442" s="11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H442" s="11" t="s">
         <v>20</v>
@@ -21656,7 +21659,7 @@
         <v>14</v>
       </c>
       <c r="G443" s="14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H443" s="14" t="s">
         <v>20</v>
@@ -21701,7 +21704,7 @@
         <v>15</v>
       </c>
       <c r="G444" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H444" s="11" t="s">
         <v>20</v>
@@ -21746,7 +21749,7 @@
         <v>16</v>
       </c>
       <c r="G445" s="14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H445" s="14" t="s">
         <v>20</v>
@@ -21791,7 +21794,7 @@
         <v>17</v>
       </c>
       <c r="G446" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H446" s="11" t="s">
         <v>20</v>
@@ -21835,7 +21838,7 @@
         <v>3</v>
       </c>
       <c r="G447" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H447" s="14" t="s">
         <v>432</v>
@@ -21870,7 +21873,7 @@
         <v>10</v>
       </c>
       <c r="D448" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D448:D991" si="3">VLOOKUP(C448, $A$2:$B$11, 2, FALSE)</f>
         <v>9</v>
       </c>
       <c r="E448" s="11" t="s">
@@ -21880,7 +21883,7 @@
         <v>3</v>
       </c>
       <c r="G448" s="11" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="H448" s="11" t="s">
         <v>356</v>
@@ -21925,7 +21928,7 @@
         <v>4</v>
       </c>
       <c r="G449" s="14" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="H449" s="14" t="s">
         <v>356</v>
@@ -21949,16 +21952,106 @@
       <c r="Y449" s="2"/>
       <c r="Z449" s="2"/>
     </row>
+    <row r="450" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A450" s="16">
+        <v>437</v>
+      </c>
+      <c r="B450" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C450" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D450" s="12">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E450" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="F450" s="11">
+        <v>5</v>
+      </c>
+      <c r="G450" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="H450" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I450" s="6"/>
+      <c r="J450" s="2"/>
+      <c r="K450" s="2"/>
+      <c r="L450" s="2"/>
+      <c r="M450" s="2"/>
+      <c r="N450" s="2"/>
+      <c r="O450" s="2"/>
+      <c r="P450" s="2"/>
+      <c r="Q450" s="2"/>
+      <c r="R450" s="2"/>
+      <c r="S450" s="2"/>
+      <c r="T450" s="2"/>
+      <c r="U450" s="2"/>
+      <c r="V450" s="2"/>
+      <c r="W450" s="2"/>
+      <c r="X450" s="2"/>
+      <c r="Y450" s="2"/>
+      <c r="Z450" s="2"/>
+    </row>
+    <row r="451" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A451" s="17">
+        <v>438</v>
+      </c>
+      <c r="B451" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C451" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D451" s="15">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="E451" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="F451" s="14">
+        <v>7</v>
+      </c>
+      <c r="G451" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="H451" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I451" s="6"/>
+      <c r="J451" s="2"/>
+      <c r="K451" s="2"/>
+      <c r="L451" s="2"/>
+      <c r="M451" s="2"/>
+      <c r="N451" s="2"/>
+      <c r="O451" s="2"/>
+      <c r="P451" s="2"/>
+      <c r="Q451" s="2"/>
+      <c r="R451" s="2"/>
+      <c r="S451" s="2"/>
+      <c r="T451" s="2"/>
+      <c r="U451" s="2"/>
+      <c r="V451" s="2"/>
+      <c r="W451" s="2"/>
+      <c r="X451" s="2"/>
+      <c r="Y451" s="2"/>
+      <c r="Z451" s="2"/>
+    </row>
   </sheetData>
   <autoFilter ref="A13:H18" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C14:C449" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C14:C451" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$2:$A$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H14:H449" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H14:H451" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Nikunj Chawla,Aaron Kandikatla,Jack Fornaro"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit or System" sqref="B14:B449" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit or System" sqref="B14:B451" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Unit,System"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Created test logs for addBallot's invalidation of ballots and added the test cases to the test case list
</commit_message>
<xml_diff>
--- a/Project2/testing/Test Case List.xlsx
+++ b/Project2/testing/Test Case List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nik312123/git/repo-Team19/Project2/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED2A0EA1-CA78-9F49-91D7-CF9E69C9DF6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1851EDD2-4B4A-EF4C-9B9D-B391B88482AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="480">
   <si>
     <t>Class Name</t>
   </si>
@@ -1443,6 +1443,24 @@
   </si>
   <si>
     <t>testMultipleImports</t>
+  </si>
+  <si>
+    <t>testParseMultipleIrFiles</t>
+  </si>
+  <si>
+    <t>testParseMultipleOplFiles</t>
+  </si>
+  <si>
+    <t>testIrMultipleFiles</t>
+  </si>
+  <si>
+    <t>testOplMultipleFiles</t>
+  </si>
+  <si>
+    <t>testAddBallotInvalidationOdd</t>
+  </si>
+  <si>
+    <t>testAddBallotInvalidationEven</t>
   </si>
   <si>
     <t>Test Case #</t>
@@ -1452,7 +1470,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1477,6 +1495,10 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1576,7 +1598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1668,6 +1690,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1928,10 +1952,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z451"/>
+  <dimension ref="A1:Z457"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A425" workbookViewId="0">
+      <selection activeCell="D458" sqref="D458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2296,7 +2320,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>12</v>
@@ -22042,16 +22066,286 @@
       <c r="Y451" s="2"/>
       <c r="Z451" s="2"/>
     </row>
+    <row r="452" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A452" s="16">
+        <v>439</v>
+      </c>
+      <c r="B452" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C452" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D452" s="12">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E452" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="F452" s="11">
+        <v>9</v>
+      </c>
+      <c r="G452" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="H452" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="I452" s="6"/>
+      <c r="J452" s="2"/>
+      <c r="K452" s="2"/>
+      <c r="L452" s="2"/>
+      <c r="M452" s="2"/>
+      <c r="N452" s="2"/>
+      <c r="O452" s="2"/>
+      <c r="P452" s="2"/>
+      <c r="Q452" s="2"/>
+      <c r="R452" s="2"/>
+      <c r="S452" s="2"/>
+      <c r="T452" s="2"/>
+      <c r="U452" s="2"/>
+      <c r="V452" s="2"/>
+      <c r="W452" s="2"/>
+      <c r="X452" s="2"/>
+      <c r="Y452" s="2"/>
+      <c r="Z452" s="2"/>
+    </row>
+    <row r="453" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A453" s="17">
+        <v>440</v>
+      </c>
+      <c r="B453" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C453" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D453" s="15">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E453" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="F453" s="14">
+        <v>10</v>
+      </c>
+      <c r="G453" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="H453" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="I453" s="6"/>
+      <c r="J453" s="2"/>
+      <c r="K453" s="2"/>
+      <c r="L453" s="2"/>
+      <c r="M453" s="2"/>
+      <c r="N453" s="2"/>
+      <c r="O453" s="2"/>
+      <c r="P453" s="2"/>
+      <c r="Q453" s="2"/>
+      <c r="R453" s="2"/>
+      <c r="S453" s="2"/>
+      <c r="T453" s="2"/>
+      <c r="U453" s="2"/>
+      <c r="V453" s="2"/>
+      <c r="W453" s="2"/>
+      <c r="X453" s="2"/>
+      <c r="Y453" s="2"/>
+      <c r="Z453" s="2"/>
+    </row>
+    <row r="454" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A454" s="16">
+        <v>441</v>
+      </c>
+      <c r="B454" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="C454" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D454" s="12">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E454" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="F454" s="11">
+        <v>18</v>
+      </c>
+      <c r="G454" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="H454" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="I454" s="6"/>
+      <c r="J454" s="2"/>
+      <c r="K454" s="2"/>
+      <c r="L454" s="2"/>
+      <c r="M454" s="2"/>
+      <c r="N454" s="2"/>
+      <c r="O454" s="2"/>
+      <c r="P454" s="2"/>
+      <c r="Q454" s="2"/>
+      <c r="R454" s="2"/>
+      <c r="S454" s="2"/>
+      <c r="T454" s="2"/>
+      <c r="U454" s="2"/>
+      <c r="V454" s="2"/>
+      <c r="W454" s="2"/>
+      <c r="X454" s="2"/>
+      <c r="Y454" s="2"/>
+      <c r="Z454" s="2"/>
+    </row>
+    <row r="455" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A455" s="17">
+        <v>442</v>
+      </c>
+      <c r="B455" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="C455" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D455" s="15">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E455" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="F455" s="14">
+        <v>19</v>
+      </c>
+      <c r="G455" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="H455" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="I455" s="6"/>
+      <c r="J455" s="2"/>
+      <c r="K455" s="2"/>
+      <c r="L455" s="2"/>
+      <c r="M455" s="2"/>
+      <c r="N455" s="2"/>
+      <c r="O455" s="2"/>
+      <c r="P455" s="2"/>
+      <c r="Q455" s="2"/>
+      <c r="R455" s="2"/>
+      <c r="S455" s="2"/>
+      <c r="T455" s="2"/>
+      <c r="U455" s="2"/>
+      <c r="V455" s="2"/>
+      <c r="W455" s="2"/>
+      <c r="X455" s="2"/>
+      <c r="Y455" s="2"/>
+      <c r="Z455" s="2"/>
+    </row>
+    <row r="456" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A456" s="16">
+        <v>443</v>
+      </c>
+      <c r="B456" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C456" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D456" s="12">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E456" s="49" t="s">
+        <v>386</v>
+      </c>
+      <c r="F456" s="49">
+        <v>10</v>
+      </c>
+      <c r="G456" s="49" t="s">
+        <v>477</v>
+      </c>
+      <c r="H456" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I456" s="6"/>
+      <c r="J456" s="2"/>
+      <c r="K456" s="2"/>
+      <c r="L456" s="2"/>
+      <c r="M456" s="2"/>
+      <c r="N456" s="2"/>
+      <c r="O456" s="2"/>
+      <c r="P456" s="2"/>
+      <c r="Q456" s="2"/>
+      <c r="R456" s="2"/>
+      <c r="S456" s="2"/>
+      <c r="T456" s="2"/>
+      <c r="U456" s="2"/>
+      <c r="V456" s="2"/>
+      <c r="W456" s="2"/>
+      <c r="X456" s="2"/>
+      <c r="Y456" s="2"/>
+      <c r="Z456" s="2"/>
+    </row>
+    <row r="457" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A457" s="17">
+        <v>444</v>
+      </c>
+      <c r="B457" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C457" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D457" s="15">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E457" s="50" t="s">
+        <v>386</v>
+      </c>
+      <c r="F457" s="50">
+        <v>11</v>
+      </c>
+      <c r="G457" s="50" t="s">
+        <v>478</v>
+      </c>
+      <c r="H457" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I457" s="6"/>
+      <c r="J457" s="2"/>
+      <c r="K457" s="2"/>
+      <c r="L457" s="2"/>
+      <c r="M457" s="2"/>
+      <c r="N457" s="2"/>
+      <c r="O457" s="2"/>
+      <c r="P457" s="2"/>
+      <c r="Q457" s="2"/>
+      <c r="R457" s="2"/>
+      <c r="S457" s="2"/>
+      <c r="T457" s="2"/>
+      <c r="U457" s="2"/>
+      <c r="V457" s="2"/>
+      <c r="W457" s="2"/>
+      <c r="X457" s="2"/>
+      <c r="Y457" s="2"/>
+      <c r="Z457" s="2"/>
+    </row>
   </sheetData>
   <autoFilter ref="A13:H18" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C14:C451" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C14:C457" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$2:$A$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H14:H451" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H14:H457" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Nikunj Chawla,Aaron Kandikatla,Jack Fornaro"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit or System" sqref="B14:B451" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Unit or System" sqref="B14:B457" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Unit,System"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>